<commit_message>
finalizing PCB, added 3D models
</commit_message>
<xml_diff>
--- a/kicad/BOM-revC.xlsx
+++ b/kicad/BOM-revC.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\Simple-GPSDO\kicad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C0EB34AE-8C35-4983-8E14-80BBE9166184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80921F16-58C6-44AD-9663-BC01FCE2D569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="1725" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-revC" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="169">
   <si>
     <t>Ref</t>
   </si>
@@ -214,9 +214,6 @@
     <t xml:space="preserve">R27, </t>
   </si>
   <si>
-    <t>65k</t>
-  </si>
-  <si>
     <t xml:space="preserve">SW1, </t>
   </si>
   <si>
@@ -506,12 +503,36 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>TAJA475K025RNJ</t>
+  </si>
+  <si>
+    <t>CRCW080564K9FKEA</t>
+  </si>
+  <si>
+    <t>64.9K</t>
+  </si>
+  <si>
+    <t>TSOT26</t>
+  </si>
+  <si>
+    <t>NRS5030T3R3MMGJ</t>
+  </si>
+  <si>
+    <t>Taiyo_Yuden_NR_50</t>
+  </si>
+  <si>
+    <t>293D106X0016A2TE3</t>
+  </si>
+  <si>
+    <t>TMCMA1C226MTRF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1018,14 +1039,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="12" applyFont="1"/>
+    <xf numFmtId="44" fontId="19" fillId="6" borderId="5" xfId="11" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="17" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="12" applyFont="1"/>
-    <xf numFmtId="44" fontId="19" fillId="6" borderId="5" xfId="11" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1381,11 +1402,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,12 +1420,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E1" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="F1" s="9">
+      <c r="E1" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="7">
         <f>SUM(G3:G70)</f>
-        <v>85.941999999999979</v>
+        <v>90.001999999999981</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1418,16 +1439,16 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1441,10 +1462,10 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="3">
         <v>0.1</v>
@@ -1464,9 +1485,18 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
+      <c r="D4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.31</v>
+      </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G56" si="0">F4*B4</f>
-        <v>0</v>
+        <f t="shared" ref="G4:G49" si="0">F4*B4</f>
+        <v>0.31</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1480,10 +1510,10 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="3">
         <v>0.12</v>
@@ -1504,10 +1534,10 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="3">
         <v>0.1</v>
@@ -1528,10 +1558,10 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" t="s">
         <v>98</v>
-      </c>
-      <c r="E7" t="s">
-        <v>99</v>
       </c>
       <c r="F7" s="3">
         <v>0.05</v>
@@ -1551,9 +1581,18 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
+      <c r="D8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.49</v>
+      </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1566,9 +1605,18 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
+      <c r="D9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.38</v>
+      </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1582,10 +1630,10 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" t="s">
         <v>100</v>
-      </c>
-      <c r="E10" t="s">
-        <v>101</v>
       </c>
       <c r="F10" s="3">
         <v>0.37</v>
@@ -1603,13 +1651,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
         <v>102</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>103</v>
-      </c>
-      <c r="E11" t="s">
-        <v>104</v>
       </c>
       <c r="F11" s="3">
         <v>0.19</v>
@@ -1627,13 +1675,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" t="s">
         <v>105</v>
       </c>
-      <c r="D12" t="s">
-        <v>106</v>
-      </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="3">
         <v>0.19</v>
@@ -1651,13 +1699,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" t="s">
         <v>107</v>
       </c>
-      <c r="D13" t="s">
-        <v>108</v>
-      </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13" s="3">
         <v>0.19</v>
@@ -1675,13 +1723,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" t="s">
         <v>109</v>
       </c>
-      <c r="D14" t="s">
-        <v>110</v>
-      </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F14" s="3">
         <v>0.45</v>
@@ -1702,10 +1750,10 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" t="s">
         <v>111</v>
-      </c>
-      <c r="E15" t="s">
-        <v>112</v>
       </c>
       <c r="F15" s="3">
         <v>0.24</v>
@@ -1726,10 +1774,10 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F16" s="3">
         <v>0.18</v>
@@ -1750,10 +1798,10 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F17" s="3">
         <v>0.76</v>
@@ -1774,10 +1822,10 @@
         <v>31</v>
       </c>
       <c r="D18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" t="s">
         <v>117</v>
-      </c>
-      <c r="E18" t="s">
-        <v>118</v>
       </c>
       <c r="F18" s="3">
         <v>0.19</v>
@@ -1798,10 +1846,10 @@
         <v>33</v>
       </c>
       <c r="D19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="F19" s="3">
         <v>0.57999999999999996</v>
@@ -1822,10 +1870,10 @@
         <v>35</v>
       </c>
       <c r="D20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="F20" s="3">
         <v>2.61</v>
@@ -1849,7 +1897,7 @@
         <v>734152980</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F21" s="3">
         <v>6.18</v>
@@ -1870,10 +1918,10 @@
         <v>39</v>
       </c>
       <c r="D22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" t="s">
         <v>124</v>
-      </c>
-      <c r="E22" t="s">
-        <v>125</v>
       </c>
       <c r="F22" s="3">
         <v>0.86</v>
@@ -1891,13 +1939,13 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="F23" s="3">
         <v>3.05</v>
@@ -1918,10 +1966,10 @@
         <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="0"/>
@@ -1939,10 +1987,10 @@
         <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="0"/>
@@ -1960,10 +2008,10 @@
         <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F26" s="3">
         <v>0.16</v>
@@ -1983,9 +2031,18 @@
       <c r="C27" t="s">
         <v>48</v>
       </c>
+      <c r="D27" t="s">
+        <v>165</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.33</v>
+      </c>
       <c r="G27" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1999,10 +2056,10 @@
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F28" s="3">
         <v>0.1</v>
@@ -2023,10 +2080,10 @@
         <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F29" s="3">
         <v>5.7000000000000002E-2</v>
@@ -2047,10 +2104,10 @@
         <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F30" s="3">
         <v>0.1</v>
@@ -2071,10 +2128,10 @@
         <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F31" s="3">
         <v>0.1</v>
@@ -2095,10 +2152,10 @@
         <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F32" s="3">
         <v>0.1</v>
@@ -2119,10 +2176,10 @@
         <v>470</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F33" s="3">
         <v>0.1</v>
@@ -2143,10 +2200,10 @@
         <v>60</v>
       </c>
       <c r="D34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F34" s="3">
         <v>0.1</v>
@@ -2167,10 +2224,10 @@
         <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F35" s="3">
         <v>0.1</v>
@@ -2188,28 +2245,37 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>163</v>
+      </c>
+      <c r="D36" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.1</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
         <v>65</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>66</v>
-      </c>
       <c r="D37" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="F37" s="3">
         <v>0.2</v>
@@ -2221,18 +2287,18 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
         <v>67</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E38" s="6"/>
+      <c r="D38" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" s="8"/>
       <c r="G38" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2240,16 +2306,16 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
         <v>69</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
       <c r="G39" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2257,16 +2323,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
         <v>71</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
       <c r="G40" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2274,19 +2340,19 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F41" s="3">
         <v>0.9</v>
@@ -2298,19 +2364,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
         <v>75</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>76</v>
-      </c>
       <c r="D42" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" t="s">
         <v>139</v>
-      </c>
-      <c r="E42" t="s">
-        <v>140</v>
       </c>
       <c r="F42" s="3">
         <v>4.08</v>
@@ -2322,19 +2388,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
         <v>77</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>78</v>
-      </c>
       <c r="D43" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>142</v>
       </c>
       <c r="F43" s="3">
         <v>0.55000000000000004</v>
@@ -2346,19 +2412,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
         <v>79</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>80</v>
-      </c>
       <c r="D44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F44" s="3">
         <v>0.57999999999999996</v>
@@ -2370,19 +2436,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D45" t="s">
+        <v>142</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="F45" s="3">
         <v>2.81</v>
@@ -2394,19 +2460,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
         <v>83</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>84</v>
-      </c>
       <c r="D46" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" t="s">
         <v>145</v>
-      </c>
-      <c r="E46" t="s">
-        <v>146</v>
       </c>
       <c r="F46" s="3">
         <v>1.99</v>
@@ -2418,34 +2484,43 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
         <v>85</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>86</v>
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0.44</v>
       </c>
       <c r="G47" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
         <v>87</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>88</v>
-      </c>
       <c r="D48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="F48" s="3">
         <v>0.33</v>
@@ -2457,19 +2532,19 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
         <v>89</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
-        <v>90</v>
-      </c>
       <c r="D49" t="s">
+        <v>148</v>
+      </c>
+      <c r="E49" t="s">
         <v>149</v>
-      </c>
-      <c r="E49" t="s">
-        <v>150</v>
       </c>
       <c r="F49" s="3">
         <v>10</v>
@@ -2480,31 +2555,31 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
+      <c r="A50" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" t="s">
         <v>152</v>
       </c>
-      <c r="D51" t="s">
-        <v>153</v>
-      </c>
       <c r="E51" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F51" s="3">
         <v>1.33</v>
@@ -2514,24 +2589,24 @@
         <v>1.33</v>
       </c>
       <c r="I51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" t="s">
         <v>155</v>
       </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D52" t="s">
-        <v>156</v>
-      </c>
       <c r="E52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F52" s="3">
         <v>21</v>
@@ -2543,19 +2618,19 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
         <v>157</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>158</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="F53" s="3">
         <v>12</v>

</xml_diff>

<commit_message>
initial work on schematic updates
</commit_message>
<xml_diff>
--- a/kicad/BOM-revC.xlsx
+++ b/kicad/BOM-revC.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\Simple-GPSDO\kicad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Simple-GPSDO\kicad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80921F16-58C6-44AD-9663-BC01FCE2D569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-revC" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="168">
   <si>
     <t>Ref</t>
   </si>
@@ -398,9 +397,6 @@
   </si>
   <si>
     <t>n/a</t>
-  </si>
-  <si>
-    <t>LB3218T330K</t>
   </si>
   <si>
     <t>CRCW080522R1FKEA</t>
@@ -532,7 +528,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1402,11 +1398,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,11 +1417,11 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E1" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F1" s="7">
         <f>SUM(G3:G70)</f>
-        <v>90.001999999999981</v>
+        <v>89.841999999999985</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1486,7 +1482,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E4" t="s">
         <v>111</v>
@@ -1582,7 +1578,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E8" t="s">
         <v>111</v>
@@ -1606,7 +1602,7 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E9" t="s">
         <v>111</v>
@@ -2007,18 +2003,12 @@
       <c r="C26" t="s">
         <v>46</v>
       </c>
-      <c r="D26" t="s">
-        <v>126</v>
-      </c>
       <c r="E26" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="3">
-        <v>0.16</v>
-      </c>
       <c r="G26" s="3">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2032,10 +2022,10 @@
         <v>48</v>
       </c>
       <c r="D27" t="s">
+        <v>164</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="F27" s="3">
         <v>0.33</v>
@@ -2056,7 +2046,7 @@
         <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>98</v>
@@ -2080,7 +2070,7 @@
         <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>98</v>
@@ -2104,7 +2094,7 @@
         <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>98</v>
@@ -2128,7 +2118,7 @@
         <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>98</v>
@@ -2152,7 +2142,7 @@
         <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>98</v>
@@ -2176,7 +2166,7 @@
         <v>470</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>98</v>
@@ -2200,7 +2190,7 @@
         <v>60</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>98</v>
@@ -2224,7 +2214,7 @@
         <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>98</v>
@@ -2245,10 +2235,10 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>98</v>
@@ -2272,10 +2262,10 @@
         <v>65</v>
       </c>
       <c r="D37" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="F37" s="3">
         <v>0.2</v>
@@ -2352,7 +2342,7 @@
         <v>73</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F41" s="3">
         <v>0.9</v>
@@ -2373,10 +2363,10 @@
         <v>75</v>
       </c>
       <c r="D42" t="s">
+        <v>137</v>
+      </c>
+      <c r="E42" t="s">
         <v>138</v>
-      </c>
-      <c r="E42" t="s">
-        <v>139</v>
       </c>
       <c r="F42" s="3">
         <v>4.08</v>
@@ -2397,10 +2387,10 @@
         <v>77</v>
       </c>
       <c r="D43" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="F43" s="3">
         <v>0.55000000000000004</v>
@@ -2424,7 +2414,7 @@
         <v>79</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F44" s="3">
         <v>0.57999999999999996</v>
@@ -2445,10 +2435,10 @@
         <v>81</v>
       </c>
       <c r="D45" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="F45" s="3">
         <v>2.81</v>
@@ -2469,10 +2459,10 @@
         <v>83</v>
       </c>
       <c r="D46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E46" t="s">
         <v>144</v>
-      </c>
-      <c r="E46" t="s">
-        <v>145</v>
       </c>
       <c r="F46" s="3">
         <v>1.99</v>
@@ -2496,7 +2486,7 @@
         <v>85</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F47" s="3">
         <v>0.44</v>
@@ -2517,10 +2507,10 @@
         <v>87</v>
       </c>
       <c r="D48" t="s">
+        <v>145</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="F48" s="3">
         <v>0.33</v>
@@ -2541,10 +2531,10 @@
         <v>89</v>
       </c>
       <c r="D49" t="s">
+        <v>147</v>
+      </c>
+      <c r="E49" t="s">
         <v>148</v>
-      </c>
-      <c r="E49" t="s">
-        <v>149</v>
       </c>
       <c r="F49" s="3">
         <v>10</v>
@@ -2556,7 +2546,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -2573,10 +2563,10 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" t="s">
         <v>151</v>
-      </c>
-      <c r="D51" t="s">
-        <v>152</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>125</v>
@@ -2589,12 +2579,12 @@
         <v>1.33</v>
       </c>
       <c r="I51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2603,7 +2593,7 @@
         <v>125</v>
       </c>
       <c r="D52" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E52" t="s">
         <v>125</v>
@@ -2618,19 +2608,19 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>155</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
         <v>156</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>157</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="F53" s="3">
         <v>12</v>

</xml_diff>